<commit_message>
grupo_cercano parallelized, added statistics to excel and determined the best option for parallelization of this function
</commit_message>
<xml_diff>
--- a/timeanalysis/Calculos tiempo.xlsx
+++ b/timeanalysis/Calculos tiempo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyanalvarez/CLionProjects/Genetica/timeanalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E77CA4B-ED11-FC4E-9C37-D26B5E3B9525}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5143A257-66AD-B846-8F68-F209B3E1DAC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="-16560" windowWidth="15040" windowHeight="15240" xr2:uid="{7930495D-EDF7-854F-A970-C65AF1ED5269}"/>
+    <workbookView xWindow="5380" yWindow="-19940" windowWidth="26240" windowHeight="16440" xr2:uid="{7930495D-EDF7-854F-A970-C65AF1ED5269}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="20">
   <si>
     <t>Serie</t>
   </si>
@@ -51,7 +51,40 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>25000 (static,2)</t>
+  </si>
+  <si>
+    <t>25000 (static,1)</t>
+  </si>
+  <si>
+    <t>1000 (static,1)</t>
+  </si>
+  <si>
+    <t>Total (static,1)</t>
+  </si>
+  <si>
+    <t>Total (static,2)</t>
+  </si>
+  <si>
+    <t>1000 (static,2)</t>
+  </si>
+  <si>
+    <t>Total (dynamic,1)</t>
+  </si>
+  <si>
+    <t>1000 (dynamic,1)</t>
+  </si>
+  <si>
+    <t>25000 (dynamic,1)</t>
+  </si>
+  <si>
+    <t>Total (dynamic,2)</t>
+  </si>
+  <si>
+    <t>1000 (dynamic,2)</t>
+  </si>
+  <si>
+    <t>25000 (dynamic,2)</t>
   </si>
 </sst>
 </file>
@@ -59,9 +92,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -79,6 +112,13 @@
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -124,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -132,13 +172,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1521,16 +1574,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>474133</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>321733</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>67733</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>50799</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>753533</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>101599</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1855,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2561641A-B8C1-2241-9A12-C989CFF7F3DD}">
-  <dimension ref="B1:I34"/>
+  <dimension ref="B1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1866,21 +1919,51 @@
     <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+    <row r="1" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="T2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AC2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
     </row>
-    <row r="3" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -1903,8 +1986,74 @@
       <c r="I4" s="1">
         <v>64</v>
       </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>2</v>
+      </c>
+      <c r="N4" s="1">
+        <v>4</v>
+      </c>
+      <c r="O4" s="1">
+        <v>8</v>
+      </c>
+      <c r="P4" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>32</v>
+      </c>
+      <c r="R4" s="1">
+        <v>64</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>4</v>
+      </c>
+      <c r="X4" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>16</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>64</v>
+      </c>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>16</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>32</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>64</v>
+      </c>
     </row>
-    <row r="5" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1917,8 +2066,44 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
+      <c r="K5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>3.194</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="T5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" s="2">
+        <v>3.194</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AC5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>3.194</v>
+      </c>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
     </row>
-    <row r="6" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1931,12 +2116,48 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
+      <c r="K6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="2">
+        <v>168.624</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="T6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="U6" s="2">
+        <v>168.624</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AC6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="2">
+        <v>168.624</v>
+      </c>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
     </row>
-    <row r="7" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.02</v>
       </c>
       <c r="D7" s="2"/>
@@ -1945,8 +2166,44 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
+      <c r="K7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="T7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AC7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
     </row>
-    <row r="8" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1959,8 +2216,44 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
+      <c r="K8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="2">
+        <v>28.809000000000001</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="T8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U8" s="2">
+        <v>28.809000000000001</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AC8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>28.809000000000001</v>
+      </c>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
     </row>
-    <row r="9" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1973,12 +2266,48 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
+      <c r="K9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="T9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U9" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AC9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
     </row>
-    <row r="10" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0</v>
       </c>
       <c r="D10" s="2"/>
@@ -1987,55 +2316,231 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
+      <c r="K10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="T10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U10" s="3">
+        <v>0</v>
+      </c>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AC10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <f>SUM(C5:C10)</f>
         <v>200.64999999999998</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <f>SUM(D5:D10)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <f t="shared" ref="E11:H11" si="0">SUM(E5:E10)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <f>SUM(I5:I10)</f>
         <v>0</v>
       </c>
+      <c r="K11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="4">
+        <f>SUM(L5:L10)</f>
+        <v>200.64999999999998</v>
+      </c>
+      <c r="M11" s="4">
+        <f>SUM(M5:M10)</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" ref="N11:Q11" si="1">SUM(N5:N10)</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="4">
+        <f>SUM(R5:R10)</f>
+        <v>0</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U11" s="4">
+        <f>SUM(U5:U10)</f>
+        <v>200.64999999999998</v>
+      </c>
+      <c r="V11" s="4">
+        <f>SUM(V5:V10)</f>
+        <v>0</v>
+      </c>
+      <c r="W11" s="4">
+        <f t="shared" ref="W11:Z11" si="2">SUM(W5:W10)</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="4">
+        <f>SUM(AA5:AA10)</f>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD11" s="4">
+        <f>SUM(AD5:AD10)</f>
+        <v>200.64999999999998</v>
+      </c>
+      <c r="AE11" s="4">
+        <f>SUM(AE5:AE10)</f>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="4">
+        <f t="shared" ref="AF11:AI11" si="3">SUM(AF5:AF10)</f>
+        <v>0</v>
+      </c>
+      <c r="AG11" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AH11" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AI11" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="4">
+        <f>SUM(AJ5:AJ10)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="3">
-        <v>1000</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+    <row r="12" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="K13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="T13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" s="6"/>
+      <c r="AC13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="6"/>
+      <c r="AJ13" s="6"/>
     </row>
-    <row r="14" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="7"/>
+      <c r="AJ14" s="7"/>
+    </row>
+    <row r="15" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>0</v>
@@ -2058,8 +2563,74 @@
       <c r="I15" s="1">
         <v>64</v>
       </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>2</v>
+      </c>
+      <c r="N15" s="1">
+        <v>4</v>
+      </c>
+      <c r="O15" s="1">
+        <v>8</v>
+      </c>
+      <c r="P15" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>32</v>
+      </c>
+      <c r="R15" s="1">
+        <v>64</v>
+      </c>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="V15" s="8">
+        <v>2</v>
+      </c>
+      <c r="W15" s="8">
+        <v>4</v>
+      </c>
+      <c r="X15" s="8">
+        <v>8</v>
+      </c>
+      <c r="Y15" s="8">
+        <v>16</v>
+      </c>
+      <c r="Z15" s="8">
+        <v>32</v>
+      </c>
+      <c r="AA15" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC15" s="8"/>
+      <c r="AD15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="8">
+        <v>2</v>
+      </c>
+      <c r="AF15" s="8">
+        <v>4</v>
+      </c>
+      <c r="AG15" s="8">
+        <v>8</v>
+      </c>
+      <c r="AH15" s="8">
+        <v>16</v>
+      </c>
+      <c r="AI15" s="8">
+        <v>32</v>
+      </c>
+      <c r="AJ15" s="8">
+        <v>64</v>
+      </c>
     </row>
-    <row r="16" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -2072,8 +2643,44 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
+      <c r="K16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="T16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U16" s="9">
+        <v>1.6E-2</v>
+      </c>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AC16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="9">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
     </row>
-    <row r="17" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
@@ -2086,12 +2693,48 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
+      <c r="K17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="T17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="U17" s="9">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AC17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD17" s="9">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
     </row>
-    <row r="18" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D18" s="2"/>
@@ -2100,8 +2743,44 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
+      <c r="K18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="T18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U18" s="10">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AC18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD18" s="10">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="9"/>
+      <c r="AJ18" s="9"/>
     </row>
-    <row r="19" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -2114,8 +2793,44 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
+      <c r="K19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="T19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="U19" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AC19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD19" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
     </row>
-    <row r="20" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
@@ -2128,12 +2843,48 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
+      <c r="K20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="T20" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="U20" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AC20" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD20" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+      <c r="AI20" s="9"/>
+      <c r="AJ20" s="9"/>
     </row>
-    <row r="21" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>0</v>
       </c>
       <c r="D21" s="2"/>
@@ -2142,55 +2893,248 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
+      <c r="K21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="T21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="U21" s="10">
+        <v>0</v>
+      </c>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AC21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD21" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="9"/>
     </row>
-    <row r="22" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <f>SUM(C16:C21)</f>
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <f>SUM(D16:D21)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="5">
-        <f t="shared" ref="E22:H22" si="1">SUM(E16:E21)</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="5">
+      <c r="E22" s="4">
+        <f t="shared" ref="E22:H22" si="4">SUM(E16:E21)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="4">
         <f>SUM(I16:I21)</f>
         <v>0</v>
       </c>
+      <c r="K22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L22" s="4">
+        <f>SUM(L16:L21)</f>
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="M22" s="4">
+        <f>SUM(M16:M21)</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="4">
+        <f t="shared" ref="N22:Q22" si="5">SUM(N16:N21)</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="4">
+        <f>SUM(R16:R21)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U22" s="9">
+        <f>SUM(U16:U21)</f>
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="V22" s="9">
+        <f>SUM(V16:V21)</f>
+        <v>0</v>
+      </c>
+      <c r="W22" s="9">
+        <f t="shared" ref="W22:Z22" si="6">SUM(W16:W21)</f>
+        <v>0</v>
+      </c>
+      <c r="X22" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="9">
+        <f>SUM(AA16:AA21)</f>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD22" s="9">
+        <f>SUM(AD16:AD21)</f>
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="AE22" s="9">
+        <f>SUM(AE16:AE21)</f>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="9">
+        <f t="shared" ref="AF22:AI22" si="7">SUM(AF16:AF21)</f>
+        <v>0</v>
+      </c>
+      <c r="AG22" s="9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH22" s="9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AI22" s="9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AJ22" s="9">
+        <f>SUM(AJ16:AJ21)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="3">
-        <v>25000</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+    <row r="23" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="7"/>
     </row>
-    <row r="25" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="K24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="T24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" s="6"/>
+      <c r="AC24" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="6"/>
+      <c r="AH24" s="6"/>
+      <c r="AI24" s="6"/>
+      <c r="AJ24" s="6"/>
+    </row>
+    <row r="25" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
+      <c r="AC25" s="7"/>
+      <c r="AD25" s="7"/>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="7"/>
+      <c r="AJ25" s="7"/>
+    </row>
+    <row r="26" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
         <v>0</v>
@@ -2213,8 +3157,74 @@
       <c r="I26" s="1">
         <v>64</v>
       </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" s="1">
+        <v>2</v>
+      </c>
+      <c r="N26" s="1">
+        <v>4</v>
+      </c>
+      <c r="O26" s="1">
+        <v>8</v>
+      </c>
+      <c r="P26" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>32</v>
+      </c>
+      <c r="R26" s="1">
+        <v>64</v>
+      </c>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="V26" s="8">
+        <v>2</v>
+      </c>
+      <c r="W26" s="8">
+        <v>4</v>
+      </c>
+      <c r="X26" s="8">
+        <v>8</v>
+      </c>
+      <c r="Y26" s="8">
+        <v>16</v>
+      </c>
+      <c r="Z26" s="8">
+        <v>32</v>
+      </c>
+      <c r="AA26" s="8">
+        <v>64</v>
+      </c>
+      <c r="AC26" s="8"/>
+      <c r="AD26" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="8">
+        <v>2</v>
+      </c>
+      <c r="AF26" s="8">
+        <v>4</v>
+      </c>
+      <c r="AG26" s="8">
+        <v>8</v>
+      </c>
+      <c r="AH26" s="8">
+        <v>16</v>
+      </c>
+      <c r="AI26" s="8">
+        <v>32</v>
+      </c>
+      <c r="AJ26" s="8">
+        <v>64</v>
+      </c>
     </row>
-    <row r="27" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2227,26 +3237,146 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
+      <c r="K27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0.379</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="T27" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U27" s="9">
+        <v>0.379</v>
+      </c>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AC27" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD27" s="9">
+        <v>0.379</v>
+      </c>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+      <c r="AG27" s="9"/>
+      <c r="AH27" s="9"/>
+      <c r="AI27" s="9"/>
+      <c r="AJ27" s="9"/>
     </row>
-    <row r="28" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="2">
         <v>7.5910000000000002</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="D28" s="2">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1.962</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1.008</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.312</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L28" s="2">
+        <v>7.5910000000000002</v>
+      </c>
+      <c r="M28" s="2">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1.962</v>
+      </c>
+      <c r="O28" s="2">
+        <v>1.008</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>0.312</v>
+      </c>
+      <c r="R28" s="2">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="T28" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="U28" s="9">
+        <v>7.5910000000000002</v>
+      </c>
+      <c r="V28" s="9">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="W28" s="9">
+        <v>1.962</v>
+      </c>
+      <c r="X28" s="9">
+        <v>1.008</v>
+      </c>
+      <c r="Y28" s="10">
+        <v>0.53</v>
+      </c>
+      <c r="Z28" s="9">
+        <v>0.312</v>
+      </c>
+      <c r="AA28" s="9">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="AC28" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD28" s="9">
+        <v>7.5910000000000002</v>
+      </c>
+      <c r="AE28" s="9">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="AF28" s="9">
+        <v>1.962</v>
+      </c>
+      <c r="AG28" s="9">
+        <v>1.008</v>
+      </c>
+      <c r="AH28" s="10">
+        <v>0.53</v>
+      </c>
+      <c r="AI28" s="9">
+        <v>0.312</v>
+      </c>
+      <c r="AJ28" s="9">
+        <v>1.1419999999999999</v>
+      </c>
     </row>
-    <row r="29" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D29" s="2"/>
@@ -2255,8 +3385,44 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
+      <c r="K29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L29" s="3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="T29" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="U29" s="10">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="9"/>
+      <c r="AA29" s="9"/>
+      <c r="AC29" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD29" s="10">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="9"/>
+      <c r="AG29" s="9"/>
+      <c r="AH29" s="9"/>
+      <c r="AI29" s="9"/>
+      <c r="AJ29" s="9"/>
     </row>
-    <row r="30" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
@@ -2269,8 +3435,44 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
+      <c r="K30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="T30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="U30" s="9">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="9"/>
+      <c r="Z30" s="9"/>
+      <c r="AA30" s="9"/>
+      <c r="AC30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD30" s="9">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="AE30" s="9"/>
+      <c r="AF30" s="9"/>
+      <c r="AG30" s="9"/>
+      <c r="AH30" s="9"/>
+      <c r="AI30" s="9"/>
+      <c r="AJ30" s="9"/>
     </row>
-    <row r="31" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
@@ -2283,12 +3485,48 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
+      <c r="K31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L31" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="T31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="U31" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+      <c r="AC31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD31" s="9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="9"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="9"/>
+      <c r="AI31" s="9"/>
+      <c r="AJ31" s="9"/>
     </row>
-    <row r="32" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>0</v>
       </c>
       <c r="D32" s="2"/>
@@ -2297,46 +3535,184 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
+      <c r="K32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L32" s="3">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="T32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="U32" s="10">
+        <v>0</v>
+      </c>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="9"/>
+      <c r="Z32" s="9"/>
+      <c r="AA32" s="9"/>
+      <c r="AC32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD32" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="9"/>
+      <c r="AG32" s="9"/>
+      <c r="AH32" s="9"/>
+      <c r="AI32" s="9"/>
+      <c r="AJ32" s="9"/>
     </row>
-    <row r="33" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="4">
         <f>SUM(C27:C32)</f>
         <v>8.5780000000000012</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="4">
         <f>SUM(D27:D32)</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="5">
-        <f t="shared" ref="E33:H33" si="2">SUM(E27:E32)</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H33" s="5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I33" s="5">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" ref="E33:H33" si="8">SUM(E27:E32)</f>
+        <v>1.962</v>
+      </c>
+      <c r="F33" s="4">
+        <f t="shared" si="8"/>
+        <v>1.008</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="8"/>
+        <v>0.53</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="8"/>
+        <v>0.312</v>
+      </c>
+      <c r="I33" s="4">
         <f>SUM(I27:I32)</f>
-        <v>0</v>
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33" s="4">
+        <f>SUM(L27:L32)</f>
+        <v>8.5780000000000012</v>
+      </c>
+      <c r="M33" s="4">
+        <f>SUM(M27:M32)</f>
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="N33" s="4">
+        <f t="shared" ref="N33:Q33" si="9">SUM(N27:N32)</f>
+        <v>1.962</v>
+      </c>
+      <c r="O33" s="4">
+        <f t="shared" si="9"/>
+        <v>1.008</v>
+      </c>
+      <c r="P33" s="4">
+        <f t="shared" si="9"/>
+        <v>0.53</v>
+      </c>
+      <c r="Q33" s="4">
+        <f t="shared" si="9"/>
+        <v>0.312</v>
+      </c>
+      <c r="R33" s="4">
+        <f>SUM(R27:R32)</f>
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="T33" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="U33" s="9">
+        <f>SUM(U27:U32)</f>
+        <v>8.5780000000000012</v>
+      </c>
+      <c r="V33" s="9">
+        <f>SUM(V27:V32)</f>
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="W33" s="9">
+        <f t="shared" ref="W33:Z33" si="10">SUM(W27:W32)</f>
+        <v>1.962</v>
+      </c>
+      <c r="X33" s="9">
+        <f t="shared" si="10"/>
+        <v>1.008</v>
+      </c>
+      <c r="Y33" s="9">
+        <f t="shared" si="10"/>
+        <v>0.53</v>
+      </c>
+      <c r="Z33" s="9">
+        <f t="shared" si="10"/>
+        <v>0.312</v>
+      </c>
+      <c r="AA33" s="9">
+        <f>SUM(AA27:AA32)</f>
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="AC33" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD33" s="9">
+        <f>SUM(AD27:AD32)</f>
+        <v>8.5780000000000012</v>
+      </c>
+      <c r="AE33" s="9">
+        <f>SUM(AE27:AE32)</f>
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="AF33" s="9">
+        <f t="shared" ref="AF33:AI33" si="11">SUM(AF27:AF32)</f>
+        <v>1.962</v>
+      </c>
+      <c r="AG33" s="9">
+        <f t="shared" si="11"/>
+        <v>1.008</v>
+      </c>
+      <c r="AH33" s="9">
+        <f t="shared" si="11"/>
+        <v>0.53</v>
+      </c>
+      <c r="AI33" s="9">
+        <f t="shared" si="11"/>
+        <v>0.312</v>
+      </c>
+      <c r="AJ33" s="9">
+        <f>SUM(AJ27:AJ32)</f>
+        <v>1.1419999999999999</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="12">
+    <mergeCell ref="T13:AA13"/>
+    <mergeCell ref="T24:AA24"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="T2:AA2"/>
+    <mergeCell ref="AC2:AJ2"/>
+    <mergeCell ref="AC13:AJ13"/>
+    <mergeCell ref="AC24:AJ24"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="B24:I24"/>
+    <mergeCell ref="K13:R13"/>
+    <mergeCell ref="K24:R24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
grupo_cercano bug fixed, calcular_densidad parallelized, added statistics to excel and determined the best option for parallelization of each function
</commit_message>
<xml_diff>
--- a/timeanalysis/Calculos tiempo.xlsx
+++ b/timeanalysis/Calculos tiempo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyanalvarez/CLionProjects/Genetica/timeanalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5143A257-66AD-B846-8F68-F209B3E1DAC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACCB673-116E-B04B-8AA6-71030C50F2D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="-19940" windowWidth="26240" windowHeight="16440" xr2:uid="{7930495D-EDF7-854F-A970-C65AF1ED5269}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{7930495D-EDF7-854F-A970-C65AF1ED5269}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
   <si>
     <t>Serie</t>
   </si>
@@ -51,13 +51,16 @@
     <t>TOTAL</t>
   </si>
   <si>
+    <t>Total (static)</t>
+  </si>
+  <si>
+    <t>25000 (static)</t>
+  </si>
+  <si>
     <t>25000 (static,2)</t>
   </si>
   <si>
     <t>25000 (static,1)</t>
-  </si>
-  <si>
-    <t>1000 (static,1)</t>
   </si>
   <si>
     <t>Total (static,1)</t>
@@ -66,22 +69,13 @@
     <t>Total (static,2)</t>
   </si>
   <si>
-    <t>1000 (static,2)</t>
-  </si>
-  <si>
     <t>Total (dynamic,1)</t>
-  </si>
-  <si>
-    <t>1000 (dynamic,1)</t>
   </si>
   <si>
     <t>25000 (dynamic,1)</t>
   </si>
   <si>
     <t>Total (dynamic,2)</t>
-  </si>
-  <si>
-    <t>1000 (dynamic,2)</t>
   </si>
   <si>
     <t>25000 (dynamic,2)</t>
@@ -94,7 +88,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -118,15 +112,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +138,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -164,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -181,9 +186,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,12 +196,41 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE8E6E6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1574,16 +1605,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>321733</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>651933</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>753533</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>101599</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>245533</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1908,21 +1939,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2561641A-B8C1-2241-9A12-C989CFF7F3DD}">
-  <dimension ref="B1:AJ34"/>
+  <dimension ref="B1:AS23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="AA4" zoomScale="115" workbookViewId="0">
+      <selection activeCell="AI18" sqref="AI18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" customWidth="1"/>
+    <col min="20" max="20" width="15.83203125" customWidth="1"/>
+    <col min="29" max="29" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1942,7 +1976,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="T2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
@@ -1952,7 +1986,7 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
       <c r="AC2" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
@@ -1961,9 +1995,19 @@
       <c r="AH2" s="5"/>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
+      <c r="AL2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
     </row>
-    <row r="3" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -2052,12 +2096,34 @@
       <c r="AJ4" s="1">
         <v>64</v>
       </c>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AO4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP4" s="1">
+        <v>8</v>
+      </c>
+      <c r="AQ4" s="1">
+        <v>16</v>
+      </c>
+      <c r="AR4" s="1">
+        <v>32</v>
+      </c>
+      <c r="AS4" s="1">
+        <v>64</v>
+      </c>
     </row>
-    <row r="5" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="10">
         <v>3.194</v>
       </c>
       <c r="D5" s="2"/>
@@ -2069,7 +2135,7 @@
       <c r="K5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="10">
         <v>3.194</v>
       </c>
       <c r="M5" s="2"/>
@@ -2081,7 +2147,7 @@
       <c r="T5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="10">
         <v>3.194</v>
       </c>
       <c r="V5" s="2"/>
@@ -2093,7 +2159,7 @@
       <c r="AC5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AD5" s="10">
         <v>3.194</v>
       </c>
       <c r="AE5" s="2"/>
@@ -2102,12 +2168,24 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
+      <c r="AL5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="10">
+        <v>3.194</v>
+      </c>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2"/>
     </row>
-    <row r="6" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="10">
         <v>168.624</v>
       </c>
       <c r="D6" s="2"/>
@@ -2119,7 +2197,7 @@
       <c r="K6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="10">
         <v>168.624</v>
       </c>
       <c r="M6" s="2"/>
@@ -2131,7 +2209,7 @@
       <c r="T6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6" s="10">
         <v>168.624</v>
       </c>
       <c r="V6" s="2"/>
@@ -2143,7 +2221,7 @@
       <c r="AC6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AD6" s="10">
         <v>168.624</v>
       </c>
       <c r="AE6" s="2"/>
@@ -2152,12 +2230,24 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
+      <c r="AL6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM6" s="10">
+        <v>168.624</v>
+      </c>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
     </row>
-    <row r="7" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="11">
         <v>0.02</v>
       </c>
       <c r="D7" s="2"/>
@@ -2169,7 +2259,7 @@
       <c r="K7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="11">
         <v>0.02</v>
       </c>
       <c r="M7" s="2"/>
@@ -2181,7 +2271,7 @@
       <c r="T7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U7" s="3">
+      <c r="U7" s="11">
         <v>0.02</v>
       </c>
       <c r="V7" s="2"/>
@@ -2193,7 +2283,7 @@
       <c r="AC7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AD7" s="3">
+      <c r="AD7" s="11">
         <v>0.02</v>
       </c>
       <c r="AE7" s="2"/>
@@ -2202,12 +2292,24 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
+      <c r="AL7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM7" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
     </row>
-    <row r="8" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="10">
         <v>28.809000000000001</v>
       </c>
       <c r="D8" s="2"/>
@@ -2219,7 +2321,7 @@
       <c r="K8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="10">
         <v>28.809000000000001</v>
       </c>
       <c r="M8" s="2"/>
@@ -2231,7 +2333,7 @@
       <c r="T8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="10">
         <v>28.809000000000001</v>
       </c>
       <c r="V8" s="2"/>
@@ -2243,7 +2345,7 @@
       <c r="AC8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AD8" s="10">
         <v>28.809000000000001</v>
       </c>
       <c r="AE8" s="2"/>
@@ -2252,12 +2354,24 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
+      <c r="AL8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM8" s="10">
+        <v>28.809000000000001</v>
+      </c>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
     </row>
-    <row r="9" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D9" s="2"/>
@@ -2269,7 +2383,7 @@
       <c r="K9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="M9" s="2"/>
@@ -2281,7 +2395,7 @@
       <c r="T9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="V9" s="2"/>
@@ -2293,7 +2407,7 @@
       <c r="AC9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AD9" s="2">
+      <c r="AD9" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="AE9" s="2"/>
@@ -2302,12 +2416,24 @@
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
       <c r="AJ9" s="2"/>
+      <c r="AL9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM9" s="10">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
     </row>
-    <row r="10" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="11">
         <v>0</v>
       </c>
       <c r="D10" s="2"/>
@@ -2319,7 +2445,7 @@
       <c r="K10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="11">
         <v>0</v>
       </c>
       <c r="M10" s="2"/>
@@ -2331,7 +2457,7 @@
       <c r="T10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U10" s="3">
+      <c r="U10" s="11">
         <v>0</v>
       </c>
       <c r="V10" s="2"/>
@@ -2343,7 +2469,7 @@
       <c r="AC10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AD10" s="3">
+      <c r="AD10" s="11">
         <v>0</v>
       </c>
       <c r="AE10" s="2"/>
@@ -2352,12 +2478,24 @@
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
+      <c r="AL10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AS10" s="2"/>
     </row>
-    <row r="11" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="12">
         <f>SUM(C5:C10)</f>
         <v>200.64999999999998</v>
       </c>
@@ -2388,7 +2526,7 @@
       <c r="K11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="12">
         <f>SUM(L5:L10)</f>
         <v>200.64999999999998</v>
       </c>
@@ -2397,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" ref="N11:Q11" si="1">SUM(N5:N10)</f>
+        <f t="shared" ref="N11:T11" si="1">SUM(N5:N10)</f>
         <v>0</v>
       </c>
       <c r="O11" s="4">
@@ -2419,7 +2557,7 @@
       <c r="T11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U11" s="4">
+      <c r="U11" s="12">
         <f>SUM(U5:U10)</f>
         <v>200.64999999999998</v>
       </c>
@@ -2428,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="W11" s="4">
-        <f t="shared" ref="W11:Z11" si="2">SUM(W5:W10)</f>
+        <f t="shared" ref="W11:AC11" si="2">SUM(W5:W10)</f>
         <v>0</v>
       </c>
       <c r="X11" s="4">
@@ -2450,7 +2588,7 @@
       <c r="AC11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AD11" s="4">
+      <c r="AD11" s="12">
         <f>SUM(AD5:AD10)</f>
         <v>200.64999999999998</v>
       </c>
@@ -2459,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="AF11" s="4">
-        <f t="shared" ref="AF11:AI11" si="3">SUM(AF5:AF10)</f>
+        <f t="shared" ref="AF11:AL11" si="3">SUM(AF5:AF10)</f>
         <v>0</v>
       </c>
       <c r="AG11" s="4">
@@ -2478,11 +2616,42 @@
         <f>SUM(AJ5:AJ10)</f>
         <v>0</v>
       </c>
+      <c r="AL11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AM11" s="12">
+        <f>SUM(AM5:AM10)</f>
+        <v>200.64999999999998</v>
+      </c>
+      <c r="AN11" s="4">
+        <f>SUM(AN5:AN10)</f>
+        <v>0</v>
+      </c>
+      <c r="AO11" s="4">
+        <f t="shared" ref="AO11:AS11" si="4">SUM(AO5:AO10)</f>
+        <v>0</v>
+      </c>
+      <c r="AP11" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AR11" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AS11" s="4">
+        <f>SUM(AS5:AS10)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2492,7 +2661,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="K13" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -2501,46 +2670,56 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
-      <c r="T13" s="6" t="s">
+      <c r="T13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+      <c r="AC13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="6"/>
-      <c r="AC13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="6"/>
-      <c r="AG13" s="6"/>
-      <c r="AH13" s="6"/>
-      <c r="AI13" s="6"/>
-      <c r="AJ13" s="6"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="5"/>
+      <c r="AI13" s="5"/>
+      <c r="AJ13" s="5"/>
+      <c r="AL13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="5"/>
+      <c r="AO13" s="5"/>
+      <c r="AP13" s="5"/>
+      <c r="AQ13" s="5"/>
+      <c r="AR13" s="5"/>
+      <c r="AS13" s="5"/>
     </row>
-    <row r="14" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="7"/>
-      <c r="AC14" s="7"/>
-      <c r="AD14" s="7"/>
-      <c r="AE14" s="7"/>
-      <c r="AF14" s="7"/>
-      <c r="AG14" s="7"/>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="7"/>
-      <c r="AJ14" s="7"/>
+    <row r="14" spans="2:45" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
+      <c r="AJ14" s="6"/>
+      <c r="AL14" s="6"/>
+      <c r="AM14" s="6"/>
+      <c r="AN14" s="6"/>
+      <c r="AO14" s="6"/>
+      <c r="AP14" s="6"/>
+      <c r="AQ14" s="6"/>
+      <c r="AR14" s="6"/>
+      <c r="AS14" s="6"/>
     </row>
-    <row r="15" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>0</v>
@@ -2585,57 +2764,79 @@
       <c r="R15" s="1">
         <v>64</v>
       </c>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="V15" s="8">
+      <c r="T15" s="1"/>
+      <c r="U15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V15" s="1">
         <v>2</v>
       </c>
-      <c r="W15" s="8">
+      <c r="W15" s="1">
         <v>4</v>
       </c>
-      <c r="X15" s="8">
+      <c r="X15" s="1">
         <v>8</v>
       </c>
-      <c r="Y15" s="8">
+      <c r="Y15" s="1">
         <v>16</v>
       </c>
-      <c r="Z15" s="8">
+      <c r="Z15" s="1">
         <v>32</v>
       </c>
-      <c r="AA15" s="8">
+      <c r="AA15" s="1">
         <v>64</v>
       </c>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE15" s="8">
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="7">
         <v>2</v>
       </c>
-      <c r="AF15" s="8">
+      <c r="AF15" s="7">
         <v>4</v>
       </c>
-      <c r="AG15" s="8">
+      <c r="AG15" s="7">
         <v>8</v>
       </c>
-      <c r="AH15" s="8">
+      <c r="AH15" s="7">
         <v>16</v>
       </c>
-      <c r="AI15" s="8">
+      <c r="AI15" s="7">
         <v>32</v>
       </c>
-      <c r="AJ15" s="8">
+      <c r="AJ15" s="7">
         <v>64</v>
       </c>
+      <c r="AL15" s="7"/>
+      <c r="AM15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="7">
+        <v>2</v>
+      </c>
+      <c r="AO15" s="7">
+        <v>4</v>
+      </c>
+      <c r="AP15" s="7">
+        <v>8</v>
+      </c>
+      <c r="AQ15" s="7">
+        <v>16</v>
+      </c>
+      <c r="AR15" s="7">
+        <v>32</v>
+      </c>
+      <c r="AS15" s="7">
+        <v>64</v>
+      </c>
     </row>
-    <row r="16" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="2">
-        <v>1.6E-2</v>
+      <c r="C16" s="10">
+        <v>0.379</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -2646,8 +2847,8 @@
       <c r="K16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L16" s="2">
-        <v>1.6E-2</v>
+      <c r="L16" s="10">
+        <v>0.379</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2655,86 +2856,170 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="T16" s="8" t="s">
+      <c r="T16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U16" s="9">
-        <v>1.6E-2</v>
-      </c>
-      <c r="V16" s="9"/>
-      <c r="W16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" s="9"/>
-      <c r="Z16" s="9"/>
-      <c r="AA16" s="9"/>
-      <c r="AC16" s="8" t="s">
+      <c r="U16" s="10">
+        <v>0.379</v>
+      </c>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AC16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="AD16" s="9">
-        <v>1.6E-2</v>
-      </c>
-      <c r="AE16" s="9"/>
-      <c r="AF16" s="9"/>
-      <c r="AG16" s="9"/>
-      <c r="AH16" s="9"/>
-      <c r="AI16" s="9"/>
-      <c r="AJ16" s="9"/>
+      <c r="AD16" s="13">
+        <v>0.379</v>
+      </c>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="8"/>
+      <c r="AI16" s="8"/>
+      <c r="AJ16" s="8"/>
+      <c r="AL16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM16" s="13">
+        <v>0.379</v>
+      </c>
+      <c r="AN16" s="8"/>
+      <c r="AO16" s="8"/>
+      <c r="AP16" s="8"/>
+      <c r="AQ16" s="8"/>
+      <c r="AR16" s="8"/>
+      <c r="AS16" s="8"/>
     </row>
-    <row r="17" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="2">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="C17" s="10">
+        <v>7.5910000000000002</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3.7629999999999999</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1.974</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="H17" s="16">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.2030000000000001</v>
+      </c>
       <c r="K17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L17" s="2">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="T17" s="8" t="s">
+      <c r="L17" s="10">
+        <v>7.5910000000000002</v>
+      </c>
+      <c r="M17" s="2">
+        <v>3.8029999999999999</v>
+      </c>
+      <c r="N17" s="2">
+        <v>1.929</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="P17" s="3">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="Q17" s="16">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="R17" s="2">
+        <v>1.135</v>
+      </c>
+      <c r="T17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U17" s="9">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="V17" s="9"/>
-      <c r="W17" s="9"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" s="9"/>
-      <c r="Z17" s="9"/>
-      <c r="AA17" s="9"/>
-      <c r="AC17" s="8" t="s">
+      <c r="U17" s="10">
+        <v>7.5910000000000002</v>
+      </c>
+      <c r="V17" s="2">
+        <v>3.7930000000000001</v>
+      </c>
+      <c r="W17" s="3">
+        <v>1.93</v>
+      </c>
+      <c r="X17" s="2">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA17" s="2">
+        <v>1.1359999999999999</v>
+      </c>
+      <c r="AC17" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="AD17" s="9">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="AE17" s="9"/>
-      <c r="AF17" s="9"/>
-      <c r="AG17" s="9"/>
-      <c r="AH17" s="9"/>
-      <c r="AI17" s="9"/>
-      <c r="AJ17" s="9"/>
+      <c r="AD17" s="13">
+        <v>7.5910000000000002</v>
+      </c>
+      <c r="AE17" s="8">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="AF17" s="8">
+        <v>1.962</v>
+      </c>
+      <c r="AG17" s="8">
+        <v>1.008</v>
+      </c>
+      <c r="AH17" s="9">
+        <v>0.53</v>
+      </c>
+      <c r="AI17" s="17">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="AJ17" s="8">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="AL17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM17" s="13">
+        <v>7.5910000000000002</v>
+      </c>
+      <c r="AN17" s="8">
+        <v>3.879</v>
+      </c>
+      <c r="AO17" s="8">
+        <v>1.925</v>
+      </c>
+      <c r="AP17" s="8">
+        <v>0.995</v>
+      </c>
+      <c r="AQ17" s="9">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="AR17" s="8">
+        <v>0.311</v>
+      </c>
+      <c r="AS17" s="9">
+        <v>1.1599999999999999</v>
+      </c>
     </row>
-    <row r="18" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="11">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D18" s="2"/>
@@ -2746,7 +3031,7 @@
       <c r="K18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18" s="11">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="M18" s="2"/>
@@ -2755,86 +3040,118 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="T18" s="8" t="s">
+      <c r="T18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U18" s="10">
+      <c r="U18" s="11">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="V18" s="9"/>
-      <c r="W18" s="9"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" s="9"/>
-      <c r="Z18" s="9"/>
-      <c r="AA18" s="9"/>
-      <c r="AC18" s="8" t="s">
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AC18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AD18" s="10">
+      <c r="AD18" s="14">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AE18" s="9"/>
-      <c r="AF18" s="9"/>
-      <c r="AG18" s="9"/>
-      <c r="AH18" s="9"/>
-      <c r="AI18" s="9"/>
-      <c r="AJ18" s="9"/>
+      <c r="AE18" s="8"/>
+      <c r="AF18" s="8"/>
+      <c r="AG18" s="8"/>
+      <c r="AH18" s="8"/>
+      <c r="AI18" s="8"/>
+      <c r="AJ18" s="8"/>
+      <c r="AL18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM18" s="14">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="AN18" s="8"/>
+      <c r="AO18" s="8"/>
+      <c r="AP18" s="8"/>
+      <c r="AQ18" s="8"/>
+      <c r="AR18" s="8"/>
+      <c r="AS18" s="8"/>
     </row>
-    <row r="19" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="2">
-        <v>1E-3</v>
+      <c r="C19" s="10">
+        <v>0.58699999999999997</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="H19" s="2">
+        <v>3.1E-2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>6.7000000000000004E-2</v>
+      </c>
       <c r="K19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L19" s="2">
-        <v>1E-3</v>
+      <c r="L19" s="10">
+        <v>0.58699999999999997</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="T19" s="8" t="s">
+      <c r="Q19" s="2">
+        <v>3.1E-2</v>
+      </c>
+      <c r="R19" s="2">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="T19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U19" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
-      <c r="AC19" s="8" t="s">
+      <c r="U19" s="10">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AC19" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AD19" s="9">
-        <v>1E-3</v>
-      </c>
-      <c r="AE19" s="9"/>
-      <c r="AF19" s="9"/>
-      <c r="AG19" s="9"/>
-      <c r="AH19" s="9"/>
-      <c r="AI19" s="9"/>
-      <c r="AJ19" s="9"/>
+      <c r="AD19" s="13">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="AE19" s="8"/>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="8"/>
+      <c r="AI19" s="8"/>
+      <c r="AJ19" s="8"/>
+      <c r="AL19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM19" s="13">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="AN19" s="8"/>
+      <c r="AO19" s="8"/>
+      <c r="AP19" s="8"/>
+      <c r="AQ19" s="8"/>
+      <c r="AR19" s="8"/>
+      <c r="AS19" s="8"/>
     </row>
-    <row r="20" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D20" s="2"/>
@@ -2846,7 +3163,7 @@
       <c r="K20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="M20" s="2"/>
@@ -2855,36 +3172,48 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
-      <c r="T20" s="8" t="s">
+      <c r="T20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U20" s="9">
+      <c r="U20" s="10">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
-      <c r="AC20" s="8" t="s">
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AC20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AD20" s="9">
+      <c r="AD20" s="13">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AE20" s="9"/>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
-      <c r="AH20" s="9"/>
-      <c r="AI20" s="9"/>
-      <c r="AJ20" s="9"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="8"/>
+      <c r="AJ20" s="8"/>
+      <c r="AL20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM20" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AN20" s="8"/>
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="8"/>
+      <c r="AQ20" s="8"/>
+      <c r="AR20" s="8"/>
+      <c r="AS20" s="8"/>
     </row>
-    <row r="21" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="11">
         <v>0</v>
       </c>
       <c r="D21" s="2"/>
@@ -2896,7 +3225,7 @@
       <c r="K21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="11">
         <v>0</v>
       </c>
       <c r="M21" s="2"/>
@@ -2905,814 +3234,230 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
-      <c r="T21" s="8" t="s">
+      <c r="T21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U21" s="10">
-        <v>0</v>
-      </c>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-      <c r="AC21" s="8" t="s">
+      <c r="U21" s="11">
+        <v>0</v>
+      </c>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AC21" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AD21" s="10">
-        <v>0</v>
-      </c>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="9"/>
-      <c r="AI21" s="9"/>
-      <c r="AJ21" s="9"/>
+      <c r="AD21" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="8"/>
+      <c r="AH21" s="8"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="8"/>
+      <c r="AL21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM21" s="14">
+        <v>0</v>
+      </c>
+      <c r="AN21" s="8"/>
+      <c r="AO21" s="8"/>
+      <c r="AP21" s="8"/>
+      <c r="AQ21" s="8"/>
+      <c r="AR21" s="8"/>
+      <c r="AS21" s="8"/>
     </row>
-    <row r="22" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="12">
         <f>SUM(C16:C21)</f>
-        <v>7.3999999999999996E-2</v>
+        <v>8.5780000000000012</v>
       </c>
       <c r="D22" s="4">
         <f>SUM(D16:D21)</f>
-        <v>0</v>
+        <v>3.7629999999999999</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" ref="E22:H22" si="4">SUM(E16:E21)</f>
-        <v>0</v>
+        <f t="shared" ref="E22:H22" si="5">SUM(E16:E21)</f>
+        <v>1.974</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.98799999999999999</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.51900000000000002</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.43799999999999994</v>
       </c>
       <c r="I22" s="4">
         <f>SUM(I16:I21)</f>
-        <v>0</v>
+        <v>1.27</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="12">
         <f>SUM(L16:L21)</f>
-        <v>7.3999999999999996E-2</v>
+        <v>8.5780000000000012</v>
       </c>
       <c r="M22" s="4">
         <f>SUM(M16:M21)</f>
-        <v>0</v>
+        <v>3.8029999999999999</v>
       </c>
       <c r="N22" s="4">
-        <f t="shared" ref="N22:Q22" si="5">SUM(N16:N21)</f>
-        <v>0</v>
+        <f t="shared" ref="N22:T22" si="6">SUM(N16:N21)</f>
+        <v>1.929</v>
       </c>
       <c r="O22" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.99199999999999999</v>
       </c>
       <c r="P22" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.52200000000000002</v>
       </c>
       <c r="Q22" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0.43700000000000006</v>
       </c>
       <c r="R22" s="4">
         <f>SUM(R16:R21)</f>
-        <v>0</v>
-      </c>
-      <c r="T22" s="8" t="s">
+        <v>1.202</v>
+      </c>
+      <c r="T22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U22" s="9">
+      <c r="U22" s="12">
         <f>SUM(U16:U21)</f>
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="V22" s="9">
+        <v>8.5780000000000012</v>
+      </c>
+      <c r="V22" s="4">
         <f>SUM(V16:V21)</f>
-        <v>0</v>
-      </c>
-      <c r="W22" s="9">
-        <f t="shared" ref="W22:Z22" si="6">SUM(W16:W21)</f>
-        <v>0</v>
-      </c>
-      <c r="X22" s="9">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Y22" s="9">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Z22" s="9">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AA22" s="9">
+        <v>3.7930000000000001</v>
+      </c>
+      <c r="W22" s="4">
+        <f t="shared" ref="W22:AC22" si="7">SUM(W16:W21)</f>
+        <v>1.93</v>
+      </c>
+      <c r="X22" s="4">
+        <f t="shared" si="7"/>
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="Y22" s="4">
+        <f t="shared" si="7"/>
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="Z22" s="4">
+        <f t="shared" si="7"/>
+        <v>0.4</v>
+      </c>
+      <c r="AA22" s="4">
         <f>SUM(AA16:AA21)</f>
-        <v>0</v>
-      </c>
-      <c r="AC22" s="8" t="s">
+        <v>1.1359999999999999</v>
+      </c>
+      <c r="AC22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AD22" s="9">
+      <c r="AD22" s="13">
         <f>SUM(AD16:AD21)</f>
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="AE22" s="9">
+        <v>8.5780000000000012</v>
+      </c>
+      <c r="AE22" s="8">
         <f>SUM(AE16:AE21)</f>
-        <v>0</v>
-      </c>
-      <c r="AF22" s="9">
-        <f t="shared" ref="AF22:AI22" si="7">SUM(AF16:AF21)</f>
-        <v>0</v>
-      </c>
-      <c r="AG22" s="9">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AH22" s="9">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AI22" s="9">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="9">
-        <f>SUM(AJ16:AJ21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
-      <c r="AA23" s="7"/>
-      <c r="AC23" s="7"/>
-      <c r="AD23" s="7"/>
-      <c r="AE23" s="7"/>
-      <c r="AF23" s="7"/>
-      <c r="AG23" s="7"/>
-      <c r="AH23" s="7"/>
-      <c r="AI23" s="7"/>
-      <c r="AJ23" s="7"/>
-    </row>
-    <row r="24" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="K24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="T24" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6"/>
-      <c r="AC24" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
-      <c r="AF24" s="6"/>
-      <c r="AG24" s="6"/>
-      <c r="AH24" s="6"/>
-      <c r="AI24" s="6"/>
-      <c r="AJ24" s="6"/>
-    </row>
-    <row r="25" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T25" s="7"/>
-      <c r="U25" s="7"/>
-      <c r="V25" s="7"/>
-      <c r="W25" s="7"/>
-      <c r="X25" s="7"/>
-      <c r="Y25" s="7"/>
-      <c r="Z25" s="7"/>
-      <c r="AA25" s="7"/>
-      <c r="AC25" s="7"/>
-      <c r="AD25" s="7"/>
-      <c r="AE25" s="7"/>
-      <c r="AF25" s="7"/>
-      <c r="AG25" s="7"/>
-      <c r="AH25" s="7"/>
-      <c r="AI25" s="7"/>
-      <c r="AJ25" s="7"/>
-    </row>
-    <row r="26" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2</v>
-      </c>
-      <c r="E26" s="1">
-        <v>4</v>
-      </c>
-      <c r="F26" s="1">
-        <v>8</v>
-      </c>
-      <c r="G26" s="1">
-        <v>16</v>
-      </c>
-      <c r="H26" s="1">
-        <v>32</v>
-      </c>
-      <c r="I26" s="1">
-        <v>64</v>
-      </c>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M26" s="1">
-        <v>2</v>
-      </c>
-      <c r="N26" s="1">
-        <v>4</v>
-      </c>
-      <c r="O26" s="1">
-        <v>8</v>
-      </c>
-      <c r="P26" s="1">
-        <v>16</v>
-      </c>
-      <c r="Q26" s="1">
-        <v>32</v>
-      </c>
-      <c r="R26" s="1">
-        <v>64</v>
-      </c>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="V26" s="8">
-        <v>2</v>
-      </c>
-      <c r="W26" s="8">
-        <v>4</v>
-      </c>
-      <c r="X26" s="8">
-        <v>8</v>
-      </c>
-      <c r="Y26" s="8">
-        <v>16</v>
-      </c>
-      <c r="Z26" s="8">
-        <v>32</v>
-      </c>
-      <c r="AA26" s="8">
-        <v>64</v>
-      </c>
-      <c r="AC26" s="8"/>
-      <c r="AD26" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE26" s="8">
-        <v>2</v>
-      </c>
-      <c r="AF26" s="8">
-        <v>4</v>
-      </c>
-      <c r="AG26" s="8">
-        <v>8</v>
-      </c>
-      <c r="AH26" s="8">
-        <v>16</v>
-      </c>
-      <c r="AI26" s="8">
-        <v>32</v>
-      </c>
-      <c r="AJ26" s="8">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2">
-        <v>0.379</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="K27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L27" s="2">
-        <v>0.379</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="T27" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="U27" s="9">
-        <v>0.379</v>
-      </c>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
-      <c r="AA27" s="9"/>
-      <c r="AC27" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD27" s="9">
-        <v>0.379</v>
-      </c>
-      <c r="AE27" s="9"/>
-      <c r="AF27" s="9"/>
-      <c r="AG27" s="9"/>
-      <c r="AH27" s="9"/>
-      <c r="AI27" s="9"/>
-      <c r="AJ27" s="9"/>
-    </row>
-    <row r="28" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="2">
-        <v>7.5910000000000002</v>
-      </c>
-      <c r="D28" s="2">
         <v>3.8239999999999998</v>
       </c>
-      <c r="E28" s="2">
+      <c r="AF22" s="8">
+        <f t="shared" ref="AF22:AL22" si="8">SUM(AF16:AF21)</f>
         <v>1.962</v>
       </c>
-      <c r="F28" s="2">
-        <v>1.008</v>
-      </c>
-      <c r="G28" s="3">
-        <v>0.53</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0.312</v>
-      </c>
-      <c r="I28" s="2">
-        <v>1.1419999999999999</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L28" s="2">
-        <v>7.5910000000000002</v>
-      </c>
-      <c r="M28" s="2">
-        <v>3.8239999999999998</v>
-      </c>
-      <c r="N28" s="2">
-        <v>1.962</v>
-      </c>
-      <c r="O28" s="2">
-        <v>1.008</v>
-      </c>
-      <c r="P28" s="3">
-        <v>0.53</v>
-      </c>
-      <c r="Q28" s="2">
-        <v>0.312</v>
-      </c>
-      <c r="R28" s="2">
-        <v>1.1419999999999999</v>
-      </c>
-      <c r="T28" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="U28" s="9">
-        <v>7.5910000000000002</v>
-      </c>
-      <c r="V28" s="9">
-        <v>3.8239999999999998</v>
-      </c>
-      <c r="W28" s="9">
-        <v>1.962</v>
-      </c>
-      <c r="X28" s="9">
-        <v>1.008</v>
-      </c>
-      <c r="Y28" s="10">
-        <v>0.53</v>
-      </c>
-      <c r="Z28" s="9">
-        <v>0.312</v>
-      </c>
-      <c r="AA28" s="9">
-        <v>1.1419999999999999</v>
-      </c>
-      <c r="AC28" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD28" s="9">
-        <v>7.5910000000000002</v>
-      </c>
-      <c r="AE28" s="9">
-        <v>3.8239999999999998</v>
-      </c>
-      <c r="AF28" s="9">
-        <v>1.962</v>
-      </c>
-      <c r="AG28" s="9">
-        <v>1.008</v>
-      </c>
-      <c r="AH28" s="10">
-        <v>0.53</v>
-      </c>
-      <c r="AI28" s="9">
-        <v>0.312</v>
-      </c>
-      <c r="AJ28" s="9">
-        <v>1.1419999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="3">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="K29" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L29" s="3">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="T29" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U29" s="10">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="9"/>
-      <c r="Y29" s="9"/>
-      <c r="Z29" s="9"/>
-      <c r="AA29" s="9"/>
-      <c r="AC29" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD29" s="10">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="AE29" s="9"/>
-      <c r="AF29" s="9"/>
-      <c r="AG29" s="9"/>
-      <c r="AH29" s="9"/>
-      <c r="AI29" s="9"/>
-      <c r="AJ29" s="9"/>
-    </row>
-    <row r="30" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0.58699999999999997</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="K30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L30" s="2">
-        <v>0.58699999999999997</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="T30" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="U30" s="9">
-        <v>0.58699999999999997</v>
-      </c>
-      <c r="V30" s="9"/>
-      <c r="W30" s="9"/>
-      <c r="X30" s="9"/>
-      <c r="Y30" s="9"/>
-      <c r="Z30" s="9"/>
-      <c r="AA30" s="9"/>
-      <c r="AC30" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD30" s="9">
-        <v>0.58699999999999997</v>
-      </c>
-      <c r="AE30" s="9"/>
-      <c r="AF30" s="9"/>
-      <c r="AG30" s="9"/>
-      <c r="AH30" s="9"/>
-      <c r="AI30" s="9"/>
-      <c r="AJ30" s="9"/>
-    </row>
-    <row r="31" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="K31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L31" s="2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="T31" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="U31" s="9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="V31" s="9"/>
-      <c r="W31" s="9"/>
-      <c r="X31" s="9"/>
-      <c r="Y31" s="9"/>
-      <c r="Z31" s="9"/>
-      <c r="AA31" s="9"/>
-      <c r="AC31" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD31" s="9">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AE31" s="9"/>
-      <c r="AF31" s="9"/>
-      <c r="AG31" s="9"/>
-      <c r="AH31" s="9"/>
-      <c r="AI31" s="9"/>
-      <c r="AJ31" s="9"/>
-    </row>
-    <row r="32" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="3">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="K32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L32" s="3">
-        <v>0</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="T32" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="U32" s="10">
-        <v>0</v>
-      </c>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-      <c r="AA32" s="9"/>
-      <c r="AC32" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD32" s="10">
-        <v>0</v>
-      </c>
-      <c r="AE32" s="9"/>
-      <c r="AF32" s="9"/>
-      <c r="AG32" s="9"/>
-      <c r="AH32" s="9"/>
-      <c r="AI32" s="9"/>
-      <c r="AJ32" s="9"/>
-    </row>
-    <row r="33" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="4">
-        <f>SUM(C27:C32)</f>
-        <v>8.5780000000000012</v>
-      </c>
-      <c r="D33" s="4">
-        <f>SUM(D27:D32)</f>
-        <v>3.8239999999999998</v>
-      </c>
-      <c r="E33" s="4">
-        <f t="shared" ref="E33:H33" si="8">SUM(E27:E32)</f>
-        <v>1.962</v>
-      </c>
-      <c r="F33" s="4">
+      <c r="AG22" s="8">
         <f t="shared" si="8"/>
         <v>1.008</v>
       </c>
-      <c r="G33" s="4">
+      <c r="AH22" s="8">
         <f t="shared" si="8"/>
         <v>0.53</v>
       </c>
-      <c r="H33" s="4">
+      <c r="AI22" s="8">
         <f t="shared" si="8"/>
-        <v>0.312</v>
-      </c>
-      <c r="I33" s="4">
-        <f>SUM(I27:I32)</f>
-        <v>1.1419999999999999</v>
-      </c>
-      <c r="K33" s="1" t="s">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="AJ22" s="8">
+        <f>SUM(AJ16:AJ21)</f>
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="AL22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L33" s="4">
-        <f>SUM(L27:L32)</f>
+      <c r="AM22" s="13">
+        <f>SUM(AM16:AM21)</f>
         <v>8.5780000000000012</v>
       </c>
-      <c r="M33" s="4">
-        <f>SUM(M27:M32)</f>
-        <v>3.8239999999999998</v>
-      </c>
-      <c r="N33" s="4">
-        <f t="shared" ref="N33:Q33" si="9">SUM(N27:N32)</f>
-        <v>1.962</v>
-      </c>
-      <c r="O33" s="4">
+      <c r="AN22" s="8">
+        <f>SUM(AN16:AN21)</f>
+        <v>3.879</v>
+      </c>
+      <c r="AO22" s="8">
+        <f t="shared" ref="AO22:AS22" si="9">SUM(AO16:AO21)</f>
+        <v>1.925</v>
+      </c>
+      <c r="AP22" s="8">
         <f t="shared" si="9"/>
-        <v>1.008</v>
-      </c>
-      <c r="P33" s="4">
+        <v>0.995</v>
+      </c>
+      <c r="AQ22" s="8">
         <f t="shared" si="9"/>
-        <v>0.53</v>
-      </c>
-      <c r="Q33" s="4">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="AR22" s="8">
         <f t="shared" si="9"/>
-        <v>0.312</v>
-      </c>
-      <c r="R33" s="4">
-        <f>SUM(R27:R32)</f>
-        <v>1.1419999999999999</v>
-      </c>
-      <c r="T33" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="U33" s="9">
-        <f>SUM(U27:U32)</f>
-        <v>8.5780000000000012</v>
-      </c>
-      <c r="V33" s="9">
-        <f>SUM(V27:V32)</f>
-        <v>3.8239999999999998</v>
-      </c>
-      <c r="W33" s="9">
-        <f t="shared" ref="W33:Z33" si="10">SUM(W27:W32)</f>
-        <v>1.962</v>
-      </c>
-      <c r="X33" s="9">
-        <f t="shared" si="10"/>
-        <v>1.008</v>
-      </c>
-      <c r="Y33" s="9">
-        <f t="shared" si="10"/>
-        <v>0.53</v>
-      </c>
-      <c r="Z33" s="9">
-        <f t="shared" si="10"/>
-        <v>0.312</v>
-      </c>
-      <c r="AA33" s="9">
-        <f>SUM(AA27:AA32)</f>
-        <v>1.1419999999999999</v>
-      </c>
-      <c r="AC33" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD33" s="9">
-        <f>SUM(AD27:AD32)</f>
-        <v>8.5780000000000012</v>
-      </c>
-      <c r="AE33" s="9">
-        <f>SUM(AE27:AE32)</f>
-        <v>3.8239999999999998</v>
-      </c>
-      <c r="AF33" s="9">
-        <f t="shared" ref="AF33:AI33" si="11">SUM(AF27:AF32)</f>
-        <v>1.962</v>
-      </c>
-      <c r="AG33" s="9">
-        <f t="shared" si="11"/>
-        <v>1.008</v>
-      </c>
-      <c r="AH33" s="9">
-        <f t="shared" si="11"/>
-        <v>0.53</v>
-      </c>
-      <c r="AI33" s="9">
-        <f t="shared" si="11"/>
-        <v>0.312</v>
-      </c>
-      <c r="AJ33" s="9">
-        <f>SUM(AJ27:AJ32)</f>
-        <v>1.1419999999999999</v>
+        <v>0.311</v>
+      </c>
+      <c r="AS22" s="8">
+        <f>SUM(AS16:AS21)</f>
+        <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="34" spans="2:36" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:45" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="6"/>
+      <c r="AI23" s="6"/>
+      <c r="AJ23" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="10">
+    <mergeCell ref="AL2:AS2"/>
+    <mergeCell ref="AL13:AS13"/>
     <mergeCell ref="T13:AA13"/>
-    <mergeCell ref="T24:AA24"/>
     <mergeCell ref="K2:R2"/>
     <mergeCell ref="T2:AA2"/>
     <mergeCell ref="AC2:AJ2"/>
     <mergeCell ref="AC13:AJ13"/>
-    <mergeCell ref="AC24:AJ24"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B24:I24"/>
     <mergeCell ref="K13:R13"/>
-    <mergeCell ref="K24:R24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>